<commit_message>
agrego los centros sin quintil y les asigno sin identificar
</commit_message>
<xml_diff>
--- a/TablasActuales/Tabla_centros_7moa9no_limpia.xlsx
+++ b/TablasActuales/Tabla_centros_7moa9no_limpia.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C254"/>
+  <dimension ref="A1:C261"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1983,46 +1983,46 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>TREINTA Y TRES</t>
+          <t>TACUAREMBO</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>sin identificar</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>227</v>
+        <v>244</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>TREINTA Y TRES</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>73</v>
+        <v>227</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>PAYSANDU</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>sin identificar</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>74</v>
+        <v>259</v>
       </c>
     </row>
     <row r="107">
@@ -2033,17 +2033,17 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>sin identificar</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>75</v>
+        <v>222</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2052,13 +2052,13 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>ROCHA</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2067,142 +2067,142 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>SORIANO</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>CERRO LARGO</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>CERRO LARGO</t>
+          <t>ROCHA</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>153</v>
+        <v>77</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>DURAZNO</t>
+          <t>SORIANO</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>160</v>
+        <v>79</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>MALDONADO</t>
+          <t>CERRO LARGO</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>117</v>
+        <v>80</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>MALDONADO</t>
+          <t>CERRO LARGO</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>179</v>
+        <v>153</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>MALDONADO</t>
+          <t>DURAZNO</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>118</v>
+        <v>160</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>RIO NEGRO</t>
+          <t>MALDONADO</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>182</v>
+        <v>117</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>RIVERA</t>
+          <t>MALDONADO</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>86</v>
+        <v>179</v>
       </c>
     </row>
     <row r="119">
@@ -2213,197 +2213,197 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>88</v>
+        <v>118</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>RIO NEGRO</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>207</v>
+        <v>182</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>RIVERA</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>144</v>
+        <v>86</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>MALDONADO</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>82</v>
+        <v>207</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>91</v>
+        <v>144</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>SAN JOSE</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>TREINTA Y TRES</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>128</v>
+        <v>83</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>CERRO LARGO</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>145</v>
+        <v>84</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>DURAZNO</t>
+          <t>SAN JOSE</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>TREINTA Y TRES</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>243</v>
+        <v>128</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>CERRO LARGO</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -2412,28 +2412,28 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>162</v>
+        <v>145</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>RIVERA</t>
+          <t>DURAZNO</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>RIVERA</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -2442,13 +2442,13 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>ROCHA</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -2457,58 +2457,58 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>106</v>
+        <v>162</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>RIVERA</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>DURAZNO</t>
+          <t>RIVERA</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>89</v>
+        <v>248</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>ROCHA</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -2517,37 +2517,37 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>92</v>
+        <v>114</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>ROCHA</t>
+          <t>DURAZNO</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="142">
@@ -2558,17 +2558,17 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>158</v>
+        <v>92</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>ROCHA</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -2577,13 +2577,13 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>210</v>
+        <v>93</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>ROCHA</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -2592,118 +2592,118 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>249</v>
+        <v>99</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>94</v>
+        <v>158</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>COLONIA</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>95</v>
+        <v>210</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>SALTO</t>
+          <t>ROCHA</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>98</v>
+        <v>249</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>FLORES</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>sin identificar</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>100</v>
+        <v>161</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>RIVERA</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>ROCHA</t>
+          <t>COLONIA</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>226</v>
+        <v>95</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>ROCHA</t>
+          <t>SALTO</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>TREINTA Y TRES</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -2712,28 +2712,28 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>RIVERA</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>173</v>
+        <v>101</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>ROCHA</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -2742,43 +2742,43 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>174</v>
+        <v>226</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>RIO NEGRO</t>
+          <t>ROCHA</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>131</v>
+        <v>102</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>TREINTA Y TRES</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>205</v>
+        <v>104</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -2787,58 +2787,58 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>134</v>
+        <v>173</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>RIVERA</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>163</v>
+        <v>174</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>COLONIA</t>
+          <t>RIO NEGRO</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>108</v>
+        <v>131</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>COLONIA</t>
+          <t>ARTIGAS</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>sin identificar</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>109</v>
+        <v>220</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -2847,97 +2847,97 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>110</v>
+        <v>205</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>LAVALLEJA</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>111</v>
+        <v>134</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>RIVERA</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>112</v>
+        <v>163</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>SORIANO</t>
+          <t>COLONIA</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>ARTIGAS</t>
+          <t>COLONIA</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>232</v>
+        <v>109</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>COLONIA</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>LAVALLEJA</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="168">
@@ -2948,227 +2948,227 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>SORIANO</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>ARTIGAS</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>120</v>
+        <v>232</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>RIO NEGRO</t>
+          <t>ARTIGAS</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>sin identificar</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>204</v>
+        <v>231</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>SALTO</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>sin identificar</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>197</v>
+        <v>246</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>TACUAREMBO</t>
+          <t>COLONIA</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>ARTIGAS</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>165</v>
+        <v>116</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>CERRO LARGO</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>DURAZNO</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>PAYSANDU</t>
+          <t>RIO NEGRO</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>126</v>
+        <v>204</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>RIO NEGRO</t>
+          <t>SALTO</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>137</v>
+        <v>197</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>TACUAREMBO</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>195</v>
+        <v>127</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>ARTIGAS</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>129</v>
+        <v>165</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>CERRO LARGO</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -3177,88 +3177,88 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>254</v>
+        <v>124</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>ROCHA</t>
+          <t>DURAZNO</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>PAYSANDU</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>RIO NEGRO</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>212</v>
+        <v>137</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>135</v>
+        <v>195</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>SALTO</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -3267,73 +3267,73 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>166</v>
+        <v>139</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>LAVALLEJA</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>224</v>
+        <v>254</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>ROCHA</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>168</v>
+        <v>132</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>TREINTA Y TRES</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>245</v>
+        <v>146</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>MALDONADO</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>143</v>
+        <v>212</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>COLONIA</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -3342,58 +3342,58 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>215</v>
+        <v>135</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>CERRO LARGO</t>
+          <t>SALTO</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>184</v>
+        <v>136</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>147</v>
+        <v>166</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>LAVALLEJA</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>159</v>
+        <v>224</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>COLONIA</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -3402,73 +3402,73 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>TREINTA Y TRES</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>190</v>
+        <v>245</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>RIVERA</t>
+          <t>MALDONADO</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>256</v>
+        <v>143</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>COLONIA</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>148</v>
+        <v>215</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>CERRO LARGO</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>149</v>
+        <v>184</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>RIVERA</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -3477,22 +3477,22 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>TREINTA Y TRES</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="205">
@@ -3507,13 +3507,13 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>237</v>
+        <v>216</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>DURAZNO</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -3522,28 +3522,28 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>241</v>
+        <v>190</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>RIVERA</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>219</v>
+        <v>256</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>PAYSANDU</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -3552,7 +3552,7 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>181</v>
+        <v>148</v>
       </c>
     </row>
     <row r="209">
@@ -3563,62 +3563,62 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>RIVERA</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>177</v>
+        <v>151</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>TREINTA Y TRES</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>167</v>
+        <v>152</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>COLONIA</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>186</v>
+        <v>237</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>ARTIGAS</t>
+          <t>DURAZNO</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -3627,43 +3627,43 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>155</v>
+        <v>241</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>CERRO LARGO</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>156</v>
+        <v>219</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>MALDONADO</t>
+          <t>PAYSANDU</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>234</v>
+        <v>181</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>MALDONADO</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -3672,88 +3672,88 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>SALTO</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>235</v>
+        <v>177</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>239</v>
+        <v>186</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>ROCHA</t>
+          <t>ARTIGAS</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>238</v>
+        <v>155</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>CERRO LARGO</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>178</v>
+        <v>156</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>MALDONADO</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -3762,28 +3762,28 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>172</v>
+        <v>234</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>SORIANO</t>
+          <t>MALDONADO</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>236</v>
+        <v>157</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>SALTO</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -3792,22 +3792,22 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>175</v>
+        <v>235</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="226">
@@ -3818,26 +3818,26 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>217</v>
+        <v>239</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>CERRO LARGO</t>
+          <t>ROCHA</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>185</v>
+        <v>238</v>
       </c>
     </row>
     <row r="228">
@@ -3848,17 +3848,17 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>228</v>
+        <v>178</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>LAVALLEJA</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -3867,253 +3867,253 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>225</v>
+        <v>172</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>SORIANO</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>180</v>
+        <v>236</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>188</v>
+        <v>176</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>189</v>
+        <v>217</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>TACUAREMBO</t>
+          <t>CERRO LARGO</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>251</v>
+        <v>185</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>193</v>
+        <v>228</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>TREINTA Y TRES</t>
+          <t>LAVALLEJA</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>198</v>
+        <v>225</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>CERRO LARGO</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>199</v>
+        <v>180</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>RIO NEGRO</t>
+          <t>CANELONES</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>257</v>
+        <v>183</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>RIVERA</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>MONTEVIDEO</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Quintil 5</t>
+          <t>Quintil 4</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>213</v>
+        <v>189</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>PAYSANDU</t>
+          <t>TACUAREMBO</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>206</v>
+        <v>251</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>ARTIGAS</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>PAYSANDU</t>
+          <t>TREINTA Y TRES</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>ARTIGAS</t>
+          <t>CERRO LARGO</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>LAVALLEJA</t>
+          <t>RIO NEGRO</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 2</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>218</v>
+        <v>257</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>PAYSANDU</t>
+          <t>RIVERA</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -4122,88 +4122,88 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>258</v>
+        <v>202</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>TACUAREMBO</t>
+          <t>MONTEVIDEO</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Quintil 1</t>
+          <t>Quintil 5</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>ARTIGAS</t>
+          <t>PAYSANDU</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Quintil 2</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>229</v>
+        <v>206</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>ARTIGAS</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Quintil 3</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>253</v>
+        <v>208</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>LAVALLEJA</t>
+          <t>PAYSANDU</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>242</v>
+        <v>211</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>SORIANO</t>
+          <t>ARTIGAS</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 1</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>247</v>
+        <v>214</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>CANELONES</t>
+          <t>LAVALLEJA</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -4212,7 +4212,7 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>240</v>
+        <v>218</v>
       </c>
     </row>
     <row r="253">
@@ -4223,25 +4223,130 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Quintil 4</t>
+          <t>Quintil 3</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
+          <t>TACUAREMBO</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Quintil 1</t>
+        </is>
+      </c>
+      <c r="C254" t="n">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>ARTIGAS</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Quintil 2</t>
+        </is>
+      </c>
+      <c r="C255" t="n">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>FLORIDA</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Quintil 3</t>
+        </is>
+      </c>
+      <c r="C256" t="n">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>LAVALLEJA</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>Quintil 4</t>
+        </is>
+      </c>
+      <c r="C257" t="n">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
           <t>SORIANO</t>
         </is>
       </c>
-      <c r="B254" t="inlineStr">
-        <is>
-          <t>Quintil 3</t>
-        </is>
-      </c>
-      <c r="C254" t="n">
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>Quintil 4</t>
+        </is>
+      </c>
+      <c r="C258" t="n">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>CANELONES</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Quintil 4</t>
+        </is>
+      </c>
+      <c r="C259" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>PAYSANDU</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Quintil 4</t>
+        </is>
+      </c>
+      <c r="C260" t="n">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>SORIANO</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Quintil 3</t>
+        </is>
+      </c>
+      <c r="C261" t="n">
         <v>260</v>
       </c>
     </row>

</xml_diff>